<commit_message>
Updated the readme to contain the name of people who helped in the project
</commit_message>
<xml_diff>
--- a/Input/Input.xlsx
+++ b/Input/Input.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="201">
   <si>
     <t>URL_ID</t>
   </si>
@@ -27,6 +27,9 @@
     <t>https://www.businessinsider.com/netflix-strategy-big-budget-action-films-big-stars-2024-4?IR=T</t>
   </si>
   <si>
+    <t>Netflix</t>
+  </si>
+  <si>
     <t>https://www.businessinsider.in/tech/news/how-netflix-is-changing-the-global-entertainment-industry/articleshow/85430648.cms</t>
   </si>
   <si>
@@ -162,6 +165,9 @@
     <t>https://www.aboutamazon.com/news/entertainment/what-you-need-to-know-about-prime-video</t>
   </si>
   <si>
+    <t>Amazon Prime</t>
+  </si>
+  <si>
     <t>https://theconversation.com/global/topics/amazon-prime-23398</t>
   </si>
   <si>
@@ -312,6 +318,9 @@
     <t>https://m.economictimes.com/industry/media/entertainment/media/jiocinema-plans-billionaire-ambani-is-asking-for-less-than-1/day-for-his-latest-disruption/articleshow/109585803.cms</t>
   </si>
   <si>
+    <t>JioCinema</t>
+  </si>
+  <si>
     <t>https://www.business-standard.com/companies/news/jiocinema-cuts-premium-subscription-fees-to-rs-1-per-day-ipl-remains-free-124042500171_1.html</t>
   </si>
   <si>
@@ -348,7 +357,7 @@
     <t>https://www.forbesindia.com/article/storyboard18/big-surge-tata-ipl-2023-on-jiocinema-gets-recordbreaking-1300-croreplus-video-views-in-first-five-weeks/84883/1</t>
   </si>
   <si>
-    <t>https://www.icicidirect.com/research/equity/blog/with-merger-consummated-jio-cinema-viacom18-seeking-to-create-ott-behemoth</t>
+    <t>https://techcrunch.com/2024/04/24/jiocinema-launches-35-cent-premium-tier-stepping-up-rivalry-with-netflix-and-prime-video/</t>
   </si>
   <si>
     <t>https://www.thehindu.com/entertainment/movies/jio-cinema-says-it-has-created-a-new-record-with-12-crore-unique-viewers/article66919099.ece</t>
@@ -453,10 +462,13 @@
     <t>https://www.mysmartprice.com/gear/entertainment/entertainment-features/jiocinema-reportedly-biggest-ott-player-in-india/</t>
   </si>
   <si>
-    <t>https://m.imdb.com/title/tt27898516/news/?ref_=tt_nwr_sm</t>
+    <t>https://books.google.co.in/books?id=Zav4EAAAQBAJ&amp;pg=PA276&amp;lpg=PA276&amp;dq=articles+on+jiocinema&amp;source=bl&amp;ots=j9s1lBTl06&amp;sig=ACfU3U04RO2TPBRzIywgFTfHflvZt96BzA&amp;hl=en&amp;sa=X&amp;ved=2ahUKEwiR2eaZgIiGAxVKwjgGHa4jAzI4MhDoAXoECAIQAw</t>
   </si>
   <si>
     <t>https://www.cnbc.com/2022/07/06/hulu-faces-existential-crisis-as-disney-decides-how-to-move-forward.html</t>
+  </si>
+  <si>
+    <t>Hulu</t>
   </si>
   <si>
     <t>https://www.cnbc.com/2019/05/14/comcast-has-agreed-to-sell-its-stake-in-hulu-in-5-years.html</t>
@@ -613,7 +625,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -624,6 +636,10 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -644,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -653,6 +669,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -873,7 +892,8 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="34.86"/>
     <col customWidth="1" min="2" max="2" width="168.86"/>
-    <col customWidth="1" min="3" max="27" width="8.71"/>
+    <col customWidth="1" min="3" max="3" width="26.0"/>
+    <col customWidth="1" min="4" max="27" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -891,12 +911,18 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="1">
         <v>2.0</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -905,7 +931,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
@@ -913,7 +942,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
@@ -921,7 +953,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
@@ -929,7 +964,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
@@ -937,7 +975,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
@@ -945,7 +986,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
@@ -953,7 +997,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
@@ -961,7 +1008,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" ht="14.25" customHeight="1">
@@ -969,7 +1019,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" ht="14.25" customHeight="1">
@@ -977,7 +1030,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="14" ht="14.25" customHeight="1">
@@ -985,7 +1041,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="15" ht="14.25" customHeight="1">
@@ -993,7 +1052,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="16" ht="14.25" customHeight="1">
@@ -1001,7 +1063,10 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" ht="14.25" customHeight="1">
@@ -1009,7 +1074,10 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" ht="14.25" customHeight="1">
@@ -1017,7 +1085,10 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" ht="14.25" customHeight="1">
@@ -1025,7 +1096,10 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" ht="14.25" customHeight="1">
@@ -1033,7 +1107,10 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="14.25" customHeight="1">
@@ -1041,7 +1118,10 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
@@ -1049,7 +1129,10 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
@@ -1057,7 +1140,10 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
@@ -1065,7 +1151,10 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
@@ -1073,7 +1162,10 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
@@ -1081,7 +1173,10 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" ht="14.25" customHeight="1">
@@ -1089,7 +1184,10 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="28" ht="14.25" customHeight="1">
@@ -1097,7 +1195,10 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="29" ht="14.25" customHeight="1">
@@ -1105,7 +1206,10 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
@@ -1113,7 +1217,10 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
@@ -1121,7 +1228,10 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
@@ -1129,7 +1239,10 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
@@ -1137,7 +1250,10 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="34" ht="14.25" customHeight="1">
@@ -1145,7 +1261,10 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="35" ht="14.25" customHeight="1">
@@ -1153,7 +1272,10 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
@@ -1161,7 +1283,10 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
@@ -1169,7 +1294,10 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="38" ht="14.25" customHeight="1">
@@ -1177,7 +1305,10 @@
         <v>37.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="39" ht="14.25" customHeight="1">
@@ -1185,7 +1316,10 @@
         <v>38.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="40" ht="14.25" customHeight="1">
@@ -1193,7 +1327,10 @@
         <v>39.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
@@ -1201,7 +1338,10 @@
         <v>40.0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
@@ -1209,7 +1349,10 @@
         <v>41.0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="43" ht="14.25" customHeight="1">
@@ -1217,7 +1360,10 @@
         <v>42.0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
@@ -1225,7 +1371,10 @@
         <v>43.0</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
@@ -1233,7 +1382,10 @@
         <v>44.0</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="46" ht="14.25" customHeight="1">
@@ -1241,7 +1393,10 @@
         <v>45.0</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="47" ht="14.25" customHeight="1">
@@ -1249,7 +1404,10 @@
         <v>46.0</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="48" ht="14.25" customHeight="1">
@@ -1257,7 +1415,10 @@
         <v>47.0</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="49" ht="14.25" customHeight="1">
@@ -1265,7 +1426,10 @@
         <v>48.0</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="50" ht="14.25" customHeight="1">
@@ -1273,7 +1437,10 @@
         <v>49.0</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="51" ht="14.25" customHeight="1">
@@ -1281,6 +1448,9 @@
         <v>50.0</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1289,7 +1459,10 @@
         <v>51.0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="53" ht="14.25" customHeight="1">
@@ -1297,7 +1470,10 @@
         <v>52.0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="54" ht="14.25" customHeight="1">
@@ -1305,6 +1481,9 @@
         <v>53.0</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1313,7 +1492,10 @@
         <v>54.0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="56" ht="14.25" customHeight="1">
@@ -1321,7 +1503,10 @@
         <v>55.0</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1">
@@ -1329,7 +1514,10 @@
         <v>56.0</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1">
@@ -1337,7 +1525,10 @@
         <v>57.0</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="59" ht="14.25" customHeight="1">
@@ -1345,7 +1536,10 @@
         <v>58.0</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="60" ht="14.25" customHeight="1">
@@ -1353,7 +1547,10 @@
         <v>59.0</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="61" ht="14.25" customHeight="1">
@@ -1361,7 +1558,10 @@
         <v>60.0</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="62" ht="14.25" customHeight="1">
@@ -1369,7 +1569,10 @@
         <v>61.0</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="63" ht="14.25" customHeight="1">
@@ -1377,7 +1580,10 @@
         <v>62.0</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="64" ht="14.25" customHeight="1">
@@ -1385,7 +1591,10 @@
         <v>63.0</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="65" ht="14.25" customHeight="1">
@@ -1393,7 +1602,10 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="66" ht="14.25" customHeight="1">
@@ -1401,7 +1613,10 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="67" ht="14.25" customHeight="1">
@@ -1409,7 +1624,10 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="68" ht="14.25" customHeight="1">
@@ -1417,7 +1635,10 @@
         <v>67.0</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="69" ht="14.25" customHeight="1">
@@ -1425,7 +1646,10 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="70" ht="14.25" customHeight="1">
@@ -1433,7 +1657,10 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="71" ht="14.25" customHeight="1">
@@ -1441,7 +1668,10 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="72" ht="14.25" customHeight="1">
@@ -1449,7 +1679,10 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="73" ht="14.25" customHeight="1">
@@ -1457,7 +1690,10 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="74" ht="14.25" customHeight="1">
@@ -1465,7 +1701,10 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="75" ht="14.25" customHeight="1">
@@ -1473,7 +1712,10 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="76" ht="14.25" customHeight="1">
@@ -1481,7 +1723,10 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="77" ht="14.25" customHeight="1">
@@ -1489,7 +1734,10 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="78" ht="14.25" customHeight="1">
@@ -1497,7 +1745,10 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="79" ht="14.25" customHeight="1">
@@ -1505,7 +1756,10 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="80" ht="14.25" customHeight="1">
@@ -1513,7 +1767,10 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="81" ht="14.25" customHeight="1">
@@ -1521,7 +1778,10 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="82" ht="14.25" customHeight="1">
@@ -1529,7 +1789,10 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="83" ht="14.25" customHeight="1">
@@ -1537,7 +1800,10 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="84" ht="14.25" customHeight="1">
@@ -1545,7 +1811,10 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="85" ht="14.25" customHeight="1">
@@ -1553,7 +1822,10 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="86" ht="14.25" customHeight="1">
@@ -1561,7 +1833,10 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="87" ht="14.25" customHeight="1">
@@ -1569,7 +1844,10 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="88" ht="14.25" customHeight="1">
@@ -1577,7 +1855,10 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="89" ht="14.25" customHeight="1">
@@ -1585,7 +1866,10 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="90" ht="14.25" customHeight="1">
@@ -1593,7 +1877,10 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="91" ht="14.25" customHeight="1">
@@ -1601,7 +1888,10 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="92" ht="14.25" customHeight="1">
@@ -1609,7 +1899,10 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="93" ht="14.25" customHeight="1">
@@ -1617,7 +1910,10 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="94" ht="14.25" customHeight="1">
@@ -1625,7 +1921,10 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="95" ht="14.25" customHeight="1">
@@ -1633,7 +1932,10 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="96" ht="14.25" customHeight="1">
@@ -1641,7 +1943,10 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="97" ht="14.25" customHeight="1">
@@ -1649,7 +1954,10 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="98" ht="14.25" customHeight="1">
@@ -1657,7 +1965,10 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="99" ht="14.25" customHeight="1">
@@ -1665,7 +1976,10 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="100" ht="14.25" customHeight="1">
@@ -1673,7 +1987,10 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="101" ht="14.25" customHeight="1">
@@ -1681,7 +1998,10 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="102" ht="14.25" customHeight="1">
@@ -1689,7 +2009,10 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="103" ht="14.25" customHeight="1">
@@ -1697,7 +2020,10 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>98</v>
+        <v>101</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="104" ht="14.25" customHeight="1">
@@ -1705,7 +2031,10 @@
         <v>103.0</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>99</v>
+        <v>102</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="105" ht="14.25" customHeight="1">
@@ -1713,6 +2042,9 @@
         <v>104.0</v>
       </c>
       <c r="B105" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C105" s="1" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1721,7 +2053,10 @@
         <v>105.0</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="107" ht="14.25" customHeight="1">
@@ -1729,7 +2064,10 @@
         <v>106.0</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>102</v>
+        <v>105</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="108" ht="14.25" customHeight="1">
@@ -1737,7 +2075,10 @@
         <v>107.0</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="109" ht="14.25" customHeight="1">
@@ -1745,7 +2086,10 @@
         <v>108.0</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="110" ht="14.25" customHeight="1">
@@ -1753,7 +2097,10 @@
         <v>109.0</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>105</v>
+        <v>108</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="111" ht="14.25" customHeight="1">
@@ -1761,7 +2108,10 @@
         <v>110.0</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>106</v>
+        <v>109</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="112" ht="14.25" customHeight="1">
@@ -1769,7 +2119,10 @@
         <v>111.0</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="113" ht="14.25" customHeight="1">
@@ -1777,7 +2130,10 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="114" ht="14.25" customHeight="1">
@@ -1785,15 +2141,21 @@
         <v>113.0</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>109</v>
+        <v>112</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="115" ht="14.25" customHeight="1">
       <c r="A115" s="1">
         <v>114.0</v>
       </c>
-      <c r="B115" s="3" t="s">
-        <v>110</v>
+      <c r="B115" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="116" ht="14.25" customHeight="1">
@@ -1801,7 +2163,10 @@
         <v>115.0</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>111</v>
+        <v>114</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="117" ht="14.25" customHeight="1">
@@ -1809,7 +2174,10 @@
         <v>116.0</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>112</v>
+        <v>115</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="118" ht="14.25" customHeight="1">
@@ -1817,7 +2185,10 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="119" ht="14.25" customHeight="1">
@@ -1825,7 +2196,10 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="120" ht="14.25" customHeight="1">
@@ -1833,7 +2207,10 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>115</v>
+        <v>118</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="121" ht="14.25" customHeight="1">
@@ -1841,7 +2218,10 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>116</v>
+        <v>119</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="122" ht="14.25" customHeight="1">
@@ -1849,7 +2229,10 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="123" ht="14.25" customHeight="1">
@@ -1857,7 +2240,10 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="124" ht="14.25" customHeight="1">
@@ -1865,7 +2251,10 @@
         <v>123.0</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="125" ht="14.25" customHeight="1">
@@ -1873,7 +2262,10 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="126" ht="14.25" customHeight="1">
@@ -1881,7 +2273,10 @@
         <v>125.0</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="127" ht="14.25" customHeight="1">
@@ -1889,7 +2284,10 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="128" ht="14.25" customHeight="1">
@@ -1897,7 +2295,10 @@
         <v>127.0</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="129" ht="14.25" customHeight="1">
@@ -1905,7 +2306,10 @@
         <v>128.0</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="130" ht="14.25" customHeight="1">
@@ -1913,7 +2317,10 @@
         <v>129.0</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="131" ht="14.25" customHeight="1">
@@ -1921,7 +2328,10 @@
         <v>130.0</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="132" ht="14.25" customHeight="1">
@@ -1929,7 +2339,10 @@
         <v>131.0</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="133" ht="14.25" customHeight="1">
@@ -1937,7 +2350,10 @@
         <v>132.0</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="134" ht="14.25" customHeight="1">
@@ -1945,7 +2361,10 @@
         <v>133.0</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="135" ht="14.25" customHeight="1">
@@ -1953,7 +2372,10 @@
         <v>134.0</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="136" ht="14.25" customHeight="1">
@@ -1961,7 +2383,10 @@
         <v>135.0</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="137" ht="14.25" customHeight="1">
@@ -1969,7 +2394,10 @@
         <v>136.0</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="138" ht="14.25" customHeight="1">
@@ -1977,7 +2405,10 @@
         <v>137.0</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="139" ht="14.25" customHeight="1">
@@ -1985,7 +2416,10 @@
         <v>138.0</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="140" ht="14.25" customHeight="1">
@@ -1993,7 +2427,10 @@
         <v>139.0</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="141" ht="14.25" customHeight="1">
@@ -2001,7 +2438,10 @@
         <v>140.0</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="142" ht="14.25" customHeight="1">
@@ -2009,7 +2449,10 @@
         <v>141.0</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="143" ht="14.25" customHeight="1">
@@ -2017,7 +2460,10 @@
         <v>142.0</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="144" ht="14.25" customHeight="1">
@@ -2025,7 +2471,10 @@
         <v>143.0</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="145" ht="14.25" customHeight="1">
@@ -2033,7 +2482,10 @@
         <v>144.0</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="146" ht="14.25" customHeight="1">
@@ -2041,7 +2493,10 @@
         <v>145.0</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="147" ht="14.25" customHeight="1">
@@ -2049,7 +2504,10 @@
         <v>146.0</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="148" ht="14.25" customHeight="1">
@@ -2057,7 +2515,10 @@
         <v>147.0</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="149" ht="14.25" customHeight="1">
@@ -2065,7 +2526,10 @@
         <v>148.0</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="150" ht="14.25" customHeight="1">
@@ -2073,7 +2537,10 @@
         <v>149.0</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="151" ht="14.25" customHeight="1">
@@ -2081,7 +2548,10 @@
         <v>150.0</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="152" ht="14.25" customHeight="1">
@@ -2089,7 +2559,10 @@
         <v>151.0</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="153" ht="14.25" customHeight="1">
@@ -2097,7 +2570,10 @@
         <v>152.0</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="154" ht="14.25" customHeight="1">
@@ -2105,7 +2581,10 @@
         <v>153.0</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="155" ht="14.25" customHeight="1">
@@ -2113,6 +2592,9 @@
         <v>154.0</v>
       </c>
       <c r="B155" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C155" s="1" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2121,7 +2603,10 @@
         <v>155.0</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="157" ht="14.25" customHeight="1">
@@ -2129,7 +2614,10 @@
         <v>156.0</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="158" ht="14.25" customHeight="1">
@@ -2137,7 +2625,10 @@
         <v>157.0</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="159" ht="14.25" customHeight="1">
@@ -2145,7 +2636,10 @@
         <v>158.0</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="160" ht="14.25" customHeight="1">
@@ -2153,7 +2647,10 @@
         <v>159.0</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="161" ht="14.25" customHeight="1">
@@ -2161,7 +2658,10 @@
         <v>160.0</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="162" ht="14.25" customHeight="1">
@@ -2169,7 +2669,10 @@
         <v>161.0</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="163" ht="14.25" customHeight="1">
@@ -2177,7 +2680,10 @@
         <v>162.0</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="164" ht="14.25" customHeight="1">
@@ -2185,7 +2691,10 @@
         <v>163.0</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="165" ht="14.25" customHeight="1">
@@ -2193,7 +2702,10 @@
         <v>164.0</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="166" ht="14.25" customHeight="1">
@@ -2201,7 +2713,10 @@
         <v>165.0</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="167" ht="14.25" customHeight="1">
@@ -2209,7 +2724,10 @@
         <v>166.0</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="168" ht="14.25" customHeight="1">
@@ -2217,7 +2735,10 @@
         <v>167.0</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="169" ht="14.25" customHeight="1">
@@ -2225,7 +2746,10 @@
         <v>168.0</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="170" ht="14.25" customHeight="1">
@@ -2233,7 +2757,10 @@
         <v>169.0</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="171" ht="14.25" customHeight="1">
@@ -2241,7 +2768,10 @@
         <v>170.0</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="172" ht="14.25" customHeight="1">
@@ -2249,7 +2779,10 @@
         <v>171.0</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="173" ht="14.25" customHeight="1">
@@ -2257,7 +2790,10 @@
         <v>172.0</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="174" ht="14.25" customHeight="1">
@@ -2265,7 +2801,10 @@
         <v>173.0</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="175" ht="14.25" customHeight="1">
@@ -2273,7 +2812,10 @@
         <v>174.0</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="176" ht="14.25" customHeight="1">
@@ -2281,7 +2823,10 @@
         <v>175.0</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="177" ht="14.25" customHeight="1">
@@ -2289,7 +2834,10 @@
         <v>176.0</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="178" ht="14.25" customHeight="1">
@@ -2297,7 +2845,10 @@
         <v>177.0</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="179" ht="14.25" customHeight="1">
@@ -2305,7 +2856,10 @@
         <v>178.0</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="180" ht="14.25" customHeight="1">
@@ -2313,7 +2867,10 @@
         <v>179.0</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="181" ht="14.25" customHeight="1">
@@ -2321,7 +2878,10 @@
         <v>180.0</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="182" ht="14.25" customHeight="1">
@@ -2329,7 +2889,10 @@
         <v>181.0</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="183" ht="14.25" customHeight="1">
@@ -2337,7 +2900,10 @@
         <v>182.0</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="184" ht="14.25" customHeight="1">
@@ -2345,7 +2911,10 @@
         <v>183.0</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="185" ht="14.25" customHeight="1">
@@ -2353,7 +2922,10 @@
         <v>184.0</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="186" ht="14.25" customHeight="1">
@@ -2361,7 +2933,7 @@
         <v>185.0</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="187" ht="14.25" customHeight="1">
@@ -2369,7 +2941,7 @@
         <v>186.0</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="188" ht="14.25" customHeight="1">
@@ -2377,7 +2949,7 @@
         <v>187.0</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="189" ht="14.25" customHeight="1">
@@ -2385,7 +2957,7 @@
         <v>188.0</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="190" ht="14.25" customHeight="1">
@@ -2393,7 +2965,7 @@
         <v>189.0</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="191" ht="14.25" customHeight="1">
@@ -2401,7 +2973,7 @@
         <v>190.0</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="192" ht="14.25" customHeight="1">
@@ -2409,7 +2981,7 @@
         <v>191.0</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="193" ht="14.25" customHeight="1">
@@ -2417,7 +2989,7 @@
         <v>192.0</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194" ht="14.25" customHeight="1">
@@ -2425,7 +2997,7 @@
         <v>193.0</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="195" ht="14.25" customHeight="1">
@@ -2433,7 +3005,7 @@
         <v>194.0</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="196" ht="14.25" customHeight="1">
@@ -2441,7 +3013,7 @@
         <v>195.0</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="197" ht="14.25" customHeight="1">
@@ -2449,7 +3021,7 @@
         <v>196.0</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="198" ht="14.25" customHeight="1">
@@ -2457,7 +3029,7 @@
         <v>197.0</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="199" ht="14.25" customHeight="1">
@@ -2465,7 +3037,7 @@
         <v>198.0</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="200" ht="14.25" customHeight="1">
@@ -2473,7 +3045,7 @@
         <v>199.0</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="201" ht="14.25" customHeight="1">
@@ -2481,7 +3053,7 @@
         <v>200.0</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="202" ht="14.25" customHeight="1"/>

</xml_diff>